<commit_message>
Update UNCOMTRADE API key
</commit_message>
<xml_diff>
--- a/all-data.xlsx
+++ b/all-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesson Pagaduan\Google Drive\git\automate-the-boring-stuff-with-python-CIN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8ABB6DD-8BCA-465C-9BCB-C693BC1A1FD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1BCC1EB-C831-49A6-9973-02A03463687A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">data!$C$1:$C$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">data!$C$1:$C$51</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="120">
   <si>
     <t>region</t>
   </si>
@@ -381,6 +381,21 @@
   </si>
   <si>
     <t>New Zealand</t>
+  </si>
+  <si>
+    <t>ITA</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>GER</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>DEU</t>
   </si>
 </sst>
 </file>
@@ -3327,10 +3342,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3734,23 +3752,22 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>117</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>118</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" t="str">
-        <f>VLOOKUP(B13,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>HKG</v>
+        <v>75</v>
+      </c>
+      <c r="D13" t="s">
+        <v>119</v>
       </c>
       <c r="E13">
-        <v>344</v>
+        <v>276</v>
       </c>
       <c r="F13" s="2">
-        <v>532</v>
+        <v>134</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>111</v>
@@ -3767,23 +3784,23 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D14" t="str">
         <f>VLOOKUP(B14,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>IND</v>
+        <v>HKG</v>
       </c>
       <c r="E14">
-        <v>699</v>
+        <v>344</v>
       </c>
       <c r="F14" s="2">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>111</v>
@@ -3800,23 +3817,23 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D15" t="str">
         <f>VLOOKUP(B15,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>IDN</v>
+        <v>IND</v>
       </c>
       <c r="E15">
-        <v>360</v>
+        <v>699</v>
       </c>
       <c r="F15" s="2">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>111</v>
@@ -3833,23 +3850,23 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="D16" t="str">
         <f>VLOOKUP(B16,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>KAZ</v>
+        <v>IDN</v>
       </c>
       <c r="E16">
-        <v>398</v>
+        <v>360</v>
       </c>
       <c r="F16" s="2">
-        <v>916</v>
+        <v>536</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>111</v>
@@ -3866,23 +3883,22 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>115</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>116</v>
       </c>
       <c r="C17" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" t="str">
-        <f>VLOOKUP(B17,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>KGZ</v>
+        <v>75</v>
+      </c>
+      <c r="D17" t="s">
+        <v>115</v>
       </c>
       <c r="E17">
-        <v>417</v>
+        <v>381</v>
       </c>
       <c r="F17" s="2">
-        <v>917</v>
+        <v>136</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>111</v>
@@ -3899,23 +3915,23 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="D18" t="str">
         <f>VLOOKUP(B18,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>KIR</v>
+        <v>KAZ</v>
       </c>
       <c r="E18">
-        <v>296</v>
+        <v>398</v>
       </c>
       <c r="F18" s="2">
-        <v>826</v>
+        <v>916</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>111</v>
@@ -3932,23 +3948,23 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="D19" t="str">
         <f>VLOOKUP(B19,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>KOR</v>
+        <v>KGZ</v>
       </c>
       <c r="E19">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="F19" s="2">
-        <v>542</v>
+        <v>917</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>111</v>
@@ -3965,23 +3981,23 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>105</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="D20" t="str">
         <f>VLOOKUP(B20,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>LAO</v>
+        <v>KIR</v>
       </c>
       <c r="E20">
-        <v>418</v>
+        <v>296</v>
       </c>
       <c r="F20" s="2">
-        <v>544</v>
+        <v>826</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>111</v>
@@ -3998,23 +4014,23 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>92</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="D21" t="str">
         <f>VLOOKUP(B21,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>MYS</v>
+        <v>KOR</v>
       </c>
       <c r="E21">
-        <v>458</v>
+        <v>410</v>
       </c>
       <c r="F21" s="2">
-        <v>548</v>
+        <v>542</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>111</v>
@@ -4031,23 +4047,23 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>105</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="D22" t="str">
         <f>VLOOKUP(B22,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>MDV</v>
+        <v>LAO</v>
       </c>
       <c r="E22">
-        <v>462</v>
+        <v>418</v>
       </c>
       <c r="F22" s="2">
-        <v>556</v>
+        <v>544</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>111</v>
@@ -4064,23 +4080,23 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="C23" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="D23" t="str">
         <f>VLOOKUP(B23,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>MNG</v>
+        <v>MYS</v>
       </c>
       <c r="E23">
-        <v>496</v>
+        <v>458</v>
       </c>
       <c r="F23" s="2">
-        <v>948</v>
+        <v>548</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>111</v>
@@ -4097,23 +4113,23 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D24" t="str">
         <f>VLOOKUP(B24,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>MMR</v>
+        <v>MDV</v>
       </c>
       <c r="E24">
-        <v>104</v>
+        <v>462</v>
       </c>
       <c r="F24" s="2">
-        <v>518</v>
+        <v>556</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>111</v>
@@ -4130,22 +4146,23 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" t="s">
-        <v>60</v>
+        <v>19</v>
+      </c>
+      <c r="D25" t="str">
+        <f>VLOOKUP(B25,[1]Sheet1!$A:$C,3,FALSE)</f>
+        <v>MNG</v>
       </c>
       <c r="E25">
-        <v>520</v>
+        <v>496</v>
       </c>
       <c r="F25" s="2">
-        <v>0</v>
+        <v>948</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>111</v>
@@ -4162,23 +4179,23 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="C26" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="D26" t="str">
         <f>VLOOKUP(B26,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>NPL</v>
+        <v>MMR</v>
       </c>
       <c r="E26">
-        <v>524</v>
+        <v>104</v>
       </c>
       <c r="F26" s="2">
-        <v>558</v>
+        <v>518</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>111</v>
@@ -4195,19 +4212,19 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C27" t="s">
         <v>52</v>
       </c>
       <c r="D27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E27">
-        <v>570</v>
+        <v>520</v>
       </c>
       <c r="F27" s="2">
         <v>0</v>
@@ -4227,22 +4244,23 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="B28" t="s">
-        <v>114</v>
+        <v>33</v>
       </c>
       <c r="C28" t="s">
-        <v>75</v>
-      </c>
-      <c r="D28" t="s">
-        <v>113</v>
+        <v>27</v>
+      </c>
+      <c r="D28" t="str">
+        <f>VLOOKUP(B28,[1]Sheet1!$A:$C,3,FALSE)</f>
+        <v>NPL</v>
       </c>
       <c r="E28">
-        <v>554</v>
+        <v>524</v>
       </c>
       <c r="F28" s="2">
-        <v>196</v>
+        <v>558</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>111</v>
@@ -4259,23 +4277,22 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="C29" t="s">
-        <v>27</v>
-      </c>
-      <c r="D29" t="str">
-        <f>VLOOKUP(B29,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>PAK</v>
+        <v>52</v>
+      </c>
+      <c r="D29" t="s">
+        <v>62</v>
       </c>
       <c r="E29">
-        <v>586</v>
+        <v>570</v>
       </c>
       <c r="F29" s="2">
-        <v>564</v>
+        <v>0</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>111</v>
@@ -4292,23 +4309,22 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="B30" t="s">
-        <v>63</v>
+        <v>114</v>
       </c>
       <c r="C30" t="s">
-        <v>52</v>
-      </c>
-      <c r="D30" t="str">
-        <f>VLOOKUP(B30,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>PLW</v>
+        <v>75</v>
+      </c>
+      <c r="D30" t="s">
+        <v>113</v>
       </c>
       <c r="E30">
-        <v>585</v>
+        <v>554</v>
       </c>
       <c r="F30" s="2">
-        <v>565</v>
+        <v>196</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>111</v>
@@ -4325,23 +4341,23 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>95</v>
+        <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D31" t="str">
         <f>VLOOKUP(B31,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>PHL</v>
+        <v>PAK</v>
       </c>
       <c r="E31">
-        <v>608</v>
+        <v>586</v>
       </c>
       <c r="F31" s="2">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>111</v>
@@ -4358,23 +4374,23 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C32" t="s">
         <v>52</v>
       </c>
       <c r="D32" t="str">
         <f>VLOOKUP(B32,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>PNG</v>
+        <v>PLW</v>
       </c>
       <c r="E32">
-        <v>598</v>
+        <v>585</v>
       </c>
       <c r="F32" s="2">
-        <v>853</v>
+        <v>565</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>111</v>
@@ -4391,23 +4407,23 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="B33" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="C33" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="D33" t="str">
         <f>VLOOKUP(B33,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>CHN</v>
+        <v>PHL</v>
       </c>
       <c r="E33">
-        <v>156</v>
+        <v>608</v>
       </c>
       <c r="F33" s="2">
-        <v>924</v>
+        <v>566</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>111</v>
@@ -4424,23 +4440,23 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="B34" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C34" t="s">
         <v>52</v>
       </c>
       <c r="D34" t="str">
         <f>VLOOKUP(B34,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>MHL</v>
+        <v>PNG</v>
       </c>
       <c r="E34">
-        <v>584</v>
+        <v>598</v>
       </c>
       <c r="F34" s="2">
-        <v>867</v>
+        <v>853</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>111</v>
@@ -4457,23 +4473,23 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="B35" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="C35" t="s">
-        <v>75</v>
+        <v>19</v>
       </c>
       <c r="D35" t="str">
         <f>VLOOKUP(B35,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>RUS</v>
+        <v>CHN</v>
       </c>
       <c r="E35">
-        <v>643</v>
+        <v>156</v>
       </c>
       <c r="F35" s="2">
-        <v>922</v>
+        <v>924</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>111</v>
@@ -4490,23 +4506,23 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="B36" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C36" t="s">
         <v>52</v>
       </c>
       <c r="D36" t="str">
         <f>VLOOKUP(B36,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>WSM</v>
+        <v>MHL</v>
       </c>
       <c r="E36">
-        <v>882</v>
+        <v>584</v>
       </c>
       <c r="F36" s="2">
-        <v>862</v>
+        <v>867</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>111</v>
@@ -4523,23 +4539,23 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="B37" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="C37" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="D37" t="str">
         <f>VLOOKUP(B37,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>SGP</v>
+        <v>RUS</v>
       </c>
       <c r="E37">
-        <v>702</v>
+        <v>643</v>
       </c>
       <c r="F37" s="2">
-        <v>576</v>
+        <v>922</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>111</v>
@@ -4556,23 +4572,23 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B38" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C38" t="s">
         <v>52</v>
       </c>
       <c r="D38" t="str">
         <f>VLOOKUP(B38,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>SLB</v>
+        <v>WSM</v>
       </c>
       <c r="E38">
-        <v>90</v>
+        <v>882</v>
       </c>
       <c r="F38" s="2">
-        <v>813</v>
+        <v>862</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>111</v>
@@ -4589,23 +4605,23 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="B39" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C39" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="D39" t="str">
         <f>VLOOKUP(B39,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>LKA</v>
+        <v>SGP</v>
       </c>
       <c r="E39">
-        <v>144</v>
+        <v>702</v>
       </c>
       <c r="F39" s="2">
-        <v>524</v>
+        <v>576</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>111</v>
@@ -4622,23 +4638,23 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B40" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="C40" t="s">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="D40" t="str">
         <f>VLOOKUP(B40,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>TJK</v>
+        <v>SLB</v>
       </c>
       <c r="E40">
-        <v>762</v>
+        <v>90</v>
       </c>
       <c r="F40" s="2">
-        <v>923</v>
+        <v>813</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>111</v>
@@ -4655,23 +4671,23 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="B41" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="C41" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D41" t="str">
         <f>VLOOKUP(B41,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>TWN</v>
+        <v>LKA</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>144</v>
       </c>
       <c r="F41" s="2">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>111</v>
@@ -4688,23 +4704,23 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>47</v>
+        <v>99</v>
       </c>
       <c r="B42" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="C42" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="D42" t="str">
         <f>VLOOKUP(B42,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>THA</v>
+        <v>TJK</v>
       </c>
       <c r="E42">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="F42" s="2">
-        <v>578</v>
+        <v>923</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>111</v>
@@ -4721,23 +4737,23 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B43" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="C43" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="D43" t="str">
         <f>VLOOKUP(B43,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>TLS</v>
+        <v>TWN</v>
       </c>
       <c r="E43">
-        <v>626</v>
+        <v>0</v>
       </c>
       <c r="F43" s="2">
-        <v>537</v>
+        <v>528</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>111</v>
@@ -4754,23 +4770,23 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C44" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="D44" t="str">
         <f>VLOOKUP(B44,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>TKM</v>
+        <v>THA</v>
       </c>
       <c r="E44">
-        <v>795</v>
+        <v>764</v>
       </c>
       <c r="F44" s="2">
-        <v>925</v>
+        <v>578</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>111</v>
@@ -4787,23 +4803,23 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="B45" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="C45" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D45" t="str">
         <f>VLOOKUP(B45,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>TON</v>
+        <v>TLS</v>
       </c>
       <c r="E45">
-        <v>776</v>
+        <v>626</v>
       </c>
       <c r="F45" s="2">
-        <v>866</v>
+        <v>537</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>111</v>
@@ -4820,23 +4836,23 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="B46" t="s">
-        <v>70</v>
+        <v>13</v>
       </c>
       <c r="C46" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="D46" t="str">
         <f>VLOOKUP(B46,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>TUV</v>
+        <v>TKM</v>
       </c>
       <c r="E46">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="F46" s="2">
-        <v>869</v>
+        <v>925</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>111</v>
@@ -4853,23 +4869,23 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="B47" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="C47" t="s">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="D47" t="str">
         <f>VLOOKUP(B47,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>UZB</v>
+        <v>TON</v>
       </c>
       <c r="E47">
-        <v>860</v>
+        <v>776</v>
       </c>
       <c r="F47" s="2">
-        <v>927</v>
+        <v>866</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>111</v>
@@ -4886,23 +4902,23 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="B48" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C48" t="s">
         <v>52</v>
       </c>
       <c r="D48" t="str">
         <f>VLOOKUP(B48,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>VUT</v>
+        <v>TUV</v>
       </c>
       <c r="E48">
-        <v>548</v>
+        <v>798</v>
       </c>
       <c r="F48" s="2">
-        <v>846</v>
+        <v>869</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>111</v>
@@ -4919,23 +4935,23 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>102</v>
+        <v>16</v>
       </c>
       <c r="B49" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="C49" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="D49" t="str">
         <f>VLOOKUP(B49,[1]Sheet1!$A:$C,3,FALSE)</f>
-        <v>VNM</v>
+        <v>UZB</v>
       </c>
       <c r="E49">
-        <v>704</v>
+        <v>860</v>
       </c>
       <c r="F49" s="2">
-        <v>582</v>
+        <v>927</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>111</v>
@@ -4950,8 +4966,74 @@
         <v>2.177</v>
       </c>
     </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>103</v>
+      </c>
+      <c r="B50" t="s">
+        <v>72</v>
+      </c>
+      <c r="C50" t="s">
+        <v>52</v>
+      </c>
+      <c r="D50" t="str">
+        <f>VLOOKUP(B50,[1]Sheet1!$A:$C,3,FALSE)</f>
+        <v>VUT</v>
+      </c>
+      <c r="E50">
+        <v>548</v>
+      </c>
+      <c r="F50" s="2">
+        <v>846</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H50">
+        <v>-4.0209999999999999</v>
+      </c>
+      <c r="I50">
+        <v>2.887</v>
+      </c>
+      <c r="J50">
+        <v>2.177</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>102</v>
+      </c>
+      <c r="B51" t="s">
+        <v>49</v>
+      </c>
+      <c r="C51" t="s">
+        <v>38</v>
+      </c>
+      <c r="D51" t="str">
+        <f>VLOOKUP(B51,[1]Sheet1!$A:$C,3,FALSE)</f>
+        <v>VNM</v>
+      </c>
+      <c r="E51">
+        <v>704</v>
+      </c>
+      <c r="F51" s="2">
+        <v>582</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H51">
+        <v>-4.0209999999999999</v>
+      </c>
+      <c r="I51">
+        <v>2.887</v>
+      </c>
+      <c r="J51">
+        <v>2.177</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="C1:C49" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="C1:C51" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>